<commit_message>
Add additional links to README.md for dashboard layout
</commit_message>
<xml_diff>
--- a/b_sample_layout/sample_layout.xlsx
+++ b/b_sample_layout/sample_layout.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlund\Documents\GitHub\group_projects\2_camp_wx_dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlund\Documents\GitHub\group_projects\2_camp_wx_dashboard\b_sample_layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1FE3106-7547-4157-8D4F-3E0F0ABD5EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{445618C6-0283-447F-B257-8F4654A5AD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="24888" windowHeight="21576" xr2:uid="{15D98B39-D87B-4DDE-A783-A5ACE43E69C2}"/>
+    <workbookView xWindow="6720" yWindow="2028" windowWidth="21264" windowHeight="22212" activeTab="1" xr2:uid="{15D98B39-D87B-4DDE-A783-A5ACE43E69C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,19 +26,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Camp Weather</t>
   </si>
   <si>
     <t>Update Forecast Button</t>
+  </si>
+  <si>
+    <t>Drop Down Menu</t>
+  </si>
+  <si>
+    <t>Current Conditions</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Winds</t>
+  </si>
+  <si>
+    <t>Precip</t>
+  </si>
+  <si>
+    <t>Etc.</t>
+  </si>
+  <si>
+    <t>Relevant Links</t>
+  </si>
+  <si>
+    <t>Full size map</t>
+  </si>
+  <si>
+    <t>Reservation link</t>
+  </si>
+  <si>
+    <t>3 pictures on carousel</t>
+  </si>
+  <si>
+    <t>Campground Map</t>
+  </si>
+  <si>
+    <t>Campsite Picture</t>
+  </si>
+  <si>
+    <t>Google map of campground wrt AZ</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3300.1659429704255!2d-110.00855468358141!3d34.19323628056787!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8728cb078988acf3%3A0x2ef0c1759f686bae!2sShow%20Low%20Lake%20Campground!5e0!3m2!1sen!2sus!4v1626551145359!5m2!1sen!2sus" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,8 +95,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,6 +129,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -91,15 +148,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,6 +336,232 @@
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>118462</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DE0BD0F-478E-48B1-97C5-3A8685D7A2F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="11529060"/>
+          <a:ext cx="6827520" cy="4019902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>122570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D84022DC-BCAB-4A1D-8BB9-E2AF89E4A8B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1897380"/>
+          <a:ext cx="8831580" cy="4511690"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>106681</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>165688</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21E5B418-5780-4FF3-A36F-91840A2AF515}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2202180" y="6758941"/>
+          <a:ext cx="6301740" cy="4448127"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>117349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="site map">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43CD8279-62BE-41CB-A2BE-1D62466158BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3535680" y="7482841"/>
+          <a:ext cx="3657600" cy="2944368"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -581,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96142258-77D5-4EE2-9358-A73D4715B8D5}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,30 +878,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -625,4 +912,118 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB87986C-938C-4A96-93DB-28452501897D}">
+  <dimension ref="A1:P46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="91.8" x14ac:dyDescent="1.65">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="P38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="P39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A33:C33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>